<commit_message>
Upgrade to django 5.1 and bootstrap 5.3 versions. Removed dependencies to django and bootstrap related packages
</commit_message>
<xml_diff>
--- a/roc/expenditure_register/templates/expenditure_register/report.xlsx
+++ b/roc/expenditure_register/templates/expenditure_register/report.xlsx
@@ -471,7 +471,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,11 +660,11 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="7" t="inlineStr">
         <is>
@@ -683,32 +683,32 @@
       </c>
       <c r="F2" s="7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2120201017</t>
         </is>
       </c>
       <c r="G2" s="7" t="n">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="H2" s="7" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="I2" s="7" t="n">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="J2" s="7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K2" s="7" t="n">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="L2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="7" t="n">
-        <v>0</v>
+        <v>51230</v>
       </c>
       <c r="N2" s="7" t="n">
-        <v>0</v>
+        <v>51230</v>
       </c>
       <c r="O2" s="7" t="n">
         <v>0</v>
@@ -717,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="Q2" s="7" t="n">
-        <v>0</v>
+        <v>18770</v>
       </c>
       <c r="R2" s="7" t="n">
         <v>0</v>
@@ -753,6 +753,1788 @@
         <v>0</v>
       </c>
       <c r="AC2" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>2120201001</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>12368</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>12368</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K3" s="7" t="n">
+        <v>12368</v>
+      </c>
+      <c r="L3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>12368</v>
+      </c>
+      <c r="R3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E4" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>2120211001</t>
+        </is>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>9000</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>9000</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K4" s="7" t="n">
+        <v>9000</v>
+      </c>
+      <c r="L4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <v>4339.83</v>
+      </c>
+      <c r="N4" s="7" t="n">
+        <v>4339.83</v>
+      </c>
+      <c r="O4" s="7" t="n">
+        <v>199.16</v>
+      </c>
+      <c r="P4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <v>4660.17</v>
+      </c>
+      <c r="R4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>2120207001</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>240420</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>241420</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K5" s="7" t="n">
+        <v>241420</v>
+      </c>
+      <c r="L5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7" t="n">
+        <v>221270.15</v>
+      </c>
+      <c r="N5" s="7" t="n">
+        <v>221270.15</v>
+      </c>
+      <c r="O5" s="7" t="n">
+        <v>950</v>
+      </c>
+      <c r="P5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="7" t="n">
+        <v>20149.85</v>
+      </c>
+      <c r="R5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D6" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F6" s="7" t="inlineStr">
+        <is>
+          <t>2130107001</t>
+        </is>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>40000</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>5793</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>45793</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K6" s="7" t="n">
+        <v>45793</v>
+      </c>
+      <c r="L6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7" t="n">
+        <v>44230.5</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <v>44230.5</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>8810.93</v>
+      </c>
+      <c r="P6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7" t="n">
+        <v>1562.5</v>
+      </c>
+      <c r="R6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D7" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E7" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>2310401004</t>
+        </is>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K7" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="L7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D8" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>2420403001</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>6000</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K8" s="7" t="n">
+        <v>6000</v>
+      </c>
+      <c r="L8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7" t="n">
+        <v>3130</v>
+      </c>
+      <c r="N8" s="7" t="n">
+        <v>3130</v>
+      </c>
+      <c r="O8" s="7" t="n">
+        <v>590</v>
+      </c>
+      <c r="P8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="7" t="n">
+        <v>2870</v>
+      </c>
+      <c r="R8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B9" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D9" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E9" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F9" s="7" t="inlineStr">
+        <is>
+          <t>2420404001</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>37000</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>40000</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K9" s="7" t="n">
+        <v>40000</v>
+      </c>
+      <c r="L9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7" t="n">
+        <v>29240.3</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>29240.3</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>4383.04</v>
+      </c>
+      <c r="P9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="7" t="n">
+        <v>10759.7</v>
+      </c>
+      <c r="R9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D10" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E10" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F10" s="7" t="inlineStr">
+        <is>
+          <t>2420403001</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>200</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K10" s="7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="L10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="7" t="n">
+        <v>1200</v>
+      </c>
+      <c r="R10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D11" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F11" s="7" t="inlineStr">
+        <is>
+          <t>3120189001</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>10500</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>10500</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K11" s="7" t="n">
+        <v>10500</v>
+      </c>
+      <c r="L11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7" t="n">
+        <v>10500</v>
+      </c>
+      <c r="N11" s="7" t="n">
+        <v>10500</v>
+      </c>
+      <c r="O11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D12" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F12" s="7" t="inlineStr">
+        <is>
+          <t>2130205001</t>
+        </is>
+      </c>
+      <c r="G12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <v>48100</v>
+      </c>
+      <c r="I12" s="7" t="n">
+        <v>48100</v>
+      </c>
+      <c r="J12" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K12" s="7" t="n">
+        <v>48100</v>
+      </c>
+      <c r="L12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7" t="n">
+        <v>34653.76</v>
+      </c>
+      <c r="N12" s="7" t="n">
+        <v>34653.76</v>
+      </c>
+      <c r="O12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="7" t="n">
+        <v>13446.24</v>
+      </c>
+      <c r="R12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B13" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D13" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E13" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F13" s="7" t="inlineStr">
+        <is>
+          <t>2390501001</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <v>8075</v>
+      </c>
+      <c r="I13" s="7" t="n">
+        <v>8075</v>
+      </c>
+      <c r="J13" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K13" s="7" t="n">
+        <v>8075</v>
+      </c>
+      <c r="L13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7" t="n">
+        <v>3347.19</v>
+      </c>
+      <c r="N13" s="7" t="n">
+        <v>3347.19</v>
+      </c>
+      <c r="O13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="7" t="n">
+        <v>4727.81</v>
+      </c>
+      <c r="R13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D14" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F14" s="7" t="inlineStr">
+        <is>
+          <t>2120202001</t>
+        </is>
+      </c>
+      <c r="G14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <v>42000</v>
+      </c>
+      <c r="I14" s="7" t="n">
+        <v>42000</v>
+      </c>
+      <c r="J14" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K14" s="7" t="n">
+        <v>42000</v>
+      </c>
+      <c r="L14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7" t="n">
+        <v>37785</v>
+      </c>
+      <c r="N14" s="7" t="n">
+        <v>37785</v>
+      </c>
+      <c r="O14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="7" t="n">
+        <v>4215</v>
+      </c>
+      <c r="R14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D15" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E15" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F15" s="7" t="inlineStr">
+        <is>
+          <t>2130202001</t>
+        </is>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>8000</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>8000</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K15" s="7" t="n">
+        <v>8000</v>
+      </c>
+      <c r="L15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7" t="n">
+        <v>4735</v>
+      </c>
+      <c r="N15" s="7" t="n">
+        <v>4735</v>
+      </c>
+      <c r="O15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="7" t="n">
+        <v>3265</v>
+      </c>
+      <c r="R15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D16" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F16" s="7" t="inlineStr">
+        <is>
+          <t>2690201001</t>
+        </is>
+      </c>
+      <c r="G16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <v>15072</v>
+      </c>
+      <c r="I16" s="7" t="n">
+        <v>15072</v>
+      </c>
+      <c r="J16" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K16" s="7" t="n">
+        <v>15072</v>
+      </c>
+      <c r="L16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7" t="n">
+        <v>3344.82</v>
+      </c>
+      <c r="N16" s="7" t="n">
+        <v>3344.82</v>
+      </c>
+      <c r="O16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="7" t="n">
+        <v>11727.18</v>
+      </c>
+      <c r="R16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D17" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E17" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F17" s="7" t="inlineStr">
+        <is>
+          <t>2260901001</t>
+        </is>
+      </c>
+      <c r="G17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <v>700</v>
+      </c>
+      <c r="I17" s="7" t="n">
+        <v>700</v>
+      </c>
+      <c r="J17" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K17" s="7" t="n">
+        <v>700</v>
+      </c>
+      <c r="L17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7" t="n">
+        <v>350</v>
+      </c>
+      <c r="N17" s="7" t="n">
+        <v>350</v>
+      </c>
+      <c r="O17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="7" t="n">
+        <v>350</v>
+      </c>
+      <c r="R17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D18" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F18" s="7" t="inlineStr">
+        <is>
+          <t>2390589001</t>
+        </is>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>4576</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>4576</v>
+      </c>
+      <c r="J18" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K18" s="7" t="n">
+        <v>4576</v>
+      </c>
+      <c r="L18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="7" t="n">
+        <v>2076</v>
+      </c>
+      <c r="N18" s="7" t="n">
+        <v>2076</v>
+      </c>
+      <c r="O18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="7" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D19" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E19" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F19" s="7" t="inlineStr">
+        <is>
+          <t>2120212001</t>
+        </is>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>7000</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>7000</v>
+      </c>
+      <c r="J19" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K19" s="7" t="n">
+        <v>7000</v>
+      </c>
+      <c r="L19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" s="7" t="n">
+        <v>5790</v>
+      </c>
+      <c r="N19" s="7" t="n">
+        <v>5790</v>
+      </c>
+      <c r="O19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="7" t="n">
+        <v>1210</v>
+      </c>
+      <c r="R19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="7" t="inlineStr">
+        <is>
+          <t>2024</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="n">
+        <v>9</v>
+      </c>
+      <c r="C20" s="7" t="inlineStr">
+        <is>
+          <t>E99</t>
+        </is>
+      </c>
+      <c r="D20" s="7" t="inlineStr">
+        <is>
+          <t>1019</t>
+        </is>
+      </c>
+      <c r="E20" s="7" t="inlineStr">
+        <is>
+          <t>206-9922000</t>
+        </is>
+      </c>
+      <c r="F20" s="7" t="inlineStr">
+        <is>
+          <t>2420407001</t>
+        </is>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>4031</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>4031</v>
+      </c>
+      <c r="J20" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="K20" s="7" t="n">
+        <v>4031</v>
+      </c>
+      <c r="L20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="7" t="n">
+        <v>4031</v>
+      </c>
+      <c r="R20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Transfer credit between accounts is complete. Graph.js is fixed. Xlsx report is fixed. No updates are supported
</commit_message>
<xml_diff>
--- a/roc/expenditure_register/templates/expenditure_register/report.xlsx
+++ b/roc/expenditure_register/templates/expenditure_register/report.xlsx
@@ -664,7 +664,7 @@
         </is>
       </c>
       <c r="B2" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="7" t="inlineStr">
         <is>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="7" t="n">
-        <v>51230</v>
+        <v>51460</v>
       </c>
       <c r="N2" s="7" t="n">
         <v>51230</v>
@@ -720,19 +720,19 @@
         <v>18770</v>
       </c>
       <c r="R2" s="7" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="S2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="T2" s="7" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="U2" s="7" t="n">
         <v>0</v>
       </c>
       <c r="V2" s="7" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="W2" s="7" t="n">
         <v>0</v>
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="B3" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="7" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B4" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7" t="inlineStr">
         <is>
@@ -903,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="7" t="n">
-        <v>4339.83</v>
+        <v>4538.99</v>
       </c>
       <c r="N4" s="7" t="n">
         <v>4339.83</v>
@@ -918,19 +918,19 @@
         <v>4660.17</v>
       </c>
       <c r="R4" s="7" t="n">
-        <v>0</v>
+        <v>199.16</v>
       </c>
       <c r="S4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="T4" s="7" t="n">
-        <v>0</v>
+        <v>199.16</v>
       </c>
       <c r="U4" s="7" t="n">
         <v>0</v>
       </c>
       <c r="V4" s="7" t="n">
-        <v>0</v>
+        <v>199.16</v>
       </c>
       <c r="W4" s="7" t="n">
         <v>0</v>
@@ -961,7 +961,7 @@
         </is>
       </c>
       <c r="B5" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
@@ -1002,7 +1002,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="7" t="n">
-        <v>221270.15</v>
+        <v>222070.15</v>
       </c>
       <c r="N5" s="7" t="n">
         <v>221270.15</v>
@@ -1017,7 +1017,7 @@
         <v>20149.85</v>
       </c>
       <c r="R5" s="7" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="S5" s="7" t="n">
         <v>0</v>
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="B6" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="B7" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="7" t="inlineStr">
         <is>
@@ -1258,7 +1258,7 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="7" t="inlineStr">
         <is>
@@ -1299,7 +1299,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="7" t="n">
-        <v>3130</v>
+        <v>3170</v>
       </c>
       <c r="N8" s="7" t="n">
         <v>3130</v>
@@ -1314,19 +1314,19 @@
         <v>2870</v>
       </c>
       <c r="R8" s="7" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="S8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="T8" s="7" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="U8" s="7" t="n">
         <v>0</v>
       </c>
       <c r="V8" s="7" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W8" s="7" t="n">
         <v>0</v>
@@ -1357,7 +1357,7 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" s="7" t="inlineStr">
         <is>
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="7" t="n">
-        <v>29240.3</v>
+        <v>30501.95</v>
       </c>
       <c r="N9" s="7" t="n">
         <v>29240.3</v>
@@ -1413,19 +1413,19 @@
         <v>10759.7</v>
       </c>
       <c r="R9" s="7" t="n">
-        <v>0</v>
+        <v>1261.65</v>
       </c>
       <c r="S9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="T9" s="7" t="n">
-        <v>0</v>
+        <v>1261.65</v>
       </c>
       <c r="U9" s="7" t="n">
         <v>0</v>
       </c>
       <c r="V9" s="7" t="n">
-        <v>0</v>
+        <v>1261.65</v>
       </c>
       <c r="W9" s="7" t="n">
         <v>0</v>
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="7" t="inlineStr">
         <is>
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="7" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="7" t="inlineStr">
         <is>
@@ -1753,7 +1753,7 @@
         </is>
       </c>
       <c r="B13" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C13" s="7" t="inlineStr">
         <is>
@@ -1794,10 +1794,10 @@
         <v>0</v>
       </c>
       <c r="M13" s="7" t="n">
-        <v>3347.19</v>
+        <v>7838.51</v>
       </c>
       <c r="N13" s="7" t="n">
-        <v>3347.19</v>
+        <v>7838.51</v>
       </c>
       <c r="O13" s="7" t="n">
         <v>0</v>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="7" t="n">
-        <v>4727.81</v>
+        <v>236.49</v>
       </c>
       <c r="R13" s="7" t="n">
         <v>0</v>
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B14" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="7" t="inlineStr">
         <is>
@@ -1951,7 +1951,7 @@
         </is>
       </c>
       <c r="B15" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="7" t="inlineStr">
         <is>
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="B16" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="7" t="inlineStr">
         <is>
@@ -2149,7 +2149,7 @@
         </is>
       </c>
       <c r="B17" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C17" s="7" t="inlineStr">
         <is>
@@ -2248,7 +2248,7 @@
         </is>
       </c>
       <c r="B18" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" s="7" t="inlineStr">
         <is>
@@ -2289,10 +2289,10 @@
         <v>0</v>
       </c>
       <c r="M18" s="7" t="n">
-        <v>2076</v>
+        <v>4576</v>
       </c>
       <c r="N18" s="7" t="n">
-        <v>2076</v>
+        <v>4576</v>
       </c>
       <c r="O18" s="7" t="n">
         <v>0</v>
@@ -2301,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="7" t="n">
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="R18" s="7" t="n">
         <v>0</v>
@@ -2347,7 +2347,7 @@
         </is>
       </c>
       <c r="B19" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="7" t="inlineStr">
         <is>
@@ -2446,7 +2446,7 @@
         </is>
       </c>
       <c r="B20" s="7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="7" t="inlineStr">
         <is>
@@ -2487,7 +2487,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="7" t="n">
-        <v>0</v>
+        <v>507.99</v>
       </c>
       <c r="N20" s="7" t="n">
         <v>0</v>
@@ -2502,19 +2502,19 @@
         <v>4031</v>
       </c>
       <c r="R20" s="7" t="n">
-        <v>0</v>
+        <v>507.99</v>
       </c>
       <c r="S20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="T20" s="7" t="n">
-        <v>0</v>
+        <v>507.99</v>
       </c>
       <c r="U20" s="7" t="n">
         <v>0</v>
       </c>
       <c r="V20" s="7" t="n">
-        <v>0</v>
+        <v>507.99</v>
       </c>
       <c r="W20" s="7" t="n">
         <v>0</v>

</xml_diff>